<commit_message>
propre 2 (prblm prix)
</commit_message>
<xml_diff>
--- a/ressources/impactCarbone.xlsx
+++ b/ressources/impactCarbone.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hazelya\PhpstormProjects\Projet_GES\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED83262-40DB-4335-8C24-450879604156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21241735-BBEC-47C5-8F7D-C5A4D66C52E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,15 +27,30 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
+    <t>Avion (court-courrier)</t>
+  </si>
+  <si>
     <t>Moto</t>
   </si>
   <si>
+    <t>Avion (moyen-courrier)</t>
+  </si>
+  <si>
+    <t>Avion (long-courrier)</t>
+  </si>
+  <si>
+    <t>Voiture thermique</t>
+  </si>
+  <si>
     <t>Bus thermique</t>
   </si>
   <si>
     <t>Scooter et moto légère</t>
   </si>
   <si>
+    <t>Voiture électrique</t>
+  </si>
+  <si>
     <t>TER</t>
   </si>
   <si>
@@ -63,37 +78,22 @@
     <t>TGV</t>
   </si>
   <si>
-    <t>Avion (court-courrier)</t>
-  </si>
-  <si>
-    <t>Avion (moyen-courrier)</t>
-  </si>
-  <si>
-    <t>Avion (long-courrier)</t>
-  </si>
-  <si>
-    <t>Voiture électrique</t>
+    <t>Vélo</t>
+  </si>
+  <si>
+    <t>Marche</t>
+  </si>
+  <si>
+    <t>prix</t>
+  </si>
+  <si>
+    <t>emissions</t>
+  </si>
+  <si>
+    <t>vitesse</t>
   </si>
   <si>
     <t>mode_transport</t>
-  </si>
-  <si>
-    <t>emissions</t>
-  </si>
-  <si>
-    <t>Vélo</t>
-  </si>
-  <si>
-    <t>Marche</t>
-  </si>
-  <si>
-    <t>Voiture thermique</t>
-  </si>
-  <si>
-    <t>prix</t>
-  </si>
-  <si>
-    <t>vitesse</t>
   </si>
 </sst>
 </file>
@@ -129,10 +129,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -419,273 +422,273 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" customWidth="1"/>
-    <col min="2" max="2" width="31.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>230</v>
       </c>
       <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2">
+        <v>0.15</v>
+      </c>
+      <c r="D2" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
       </c>
       <c r="B3" s="1">
         <v>192</v>
       </c>
       <c r="C3" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="D3">
-        <v>53</v>
+        <v>0.13</v>
+      </c>
+      <c r="D3" s="1">
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
+      <c r="A4" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>178</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>800</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
+      <c r="A5" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>152</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+        <v>0.08</v>
+      </c>
+      <c r="D5" s="1">
+        <v>900</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
+      <c r="A6" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>136</v>
       </c>
       <c r="C6" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="D6">
-        <v>43</v>
+        <v>0.33</v>
+      </c>
+      <c r="D6" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
+      <c r="A7" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>112</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
+      <c r="A8" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>76</v>
       </c>
       <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+        <v>0.13</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
+      <c r="A9" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>65</v>
       </c>
       <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
+        <v>0.27</v>
+      </c>
+      <c r="D9" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>3</v>
+      <c r="A10" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>29</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
+        <v>0.15</v>
+      </c>
+      <c r="D10" s="1">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>4</v>
+      <c r="A11" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>29</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
+        <v>0.05</v>
+      </c>
+      <c r="D11" s="1">
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>5</v>
+      <c r="A12" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>10</v>
       </c>
       <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="1">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
+      <c r="A13" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>10</v>
       </c>
       <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
+        <v>0.02</v>
+      </c>
+      <c r="D13" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
+      <c r="A14" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>7</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
+        <v>0.12</v>
+      </c>
+      <c r="D14" s="1">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>8</v>
+      <c r="A15" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B15" s="1">
         <v>6</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>9</v>
+      <c r="A16" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
+        <v>0.12</v>
+      </c>
+      <c r="D16" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>10</v>
+      <c r="A17" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>11</v>
+      <c r="A18" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
+        <v>0.15</v>
+      </c>
+      <c r="D18" s="1">
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
+      <c r="A19" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -693,13 +696,13 @@
       <c r="C19" s="1">
         <v>0</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
+      <c r="A20" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -707,7 +710,7 @@
       <c r="C20" s="1">
         <v>0</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>